<commit_message>
Fixed data conversion error for blank values passed in excel
</commit_message>
<xml_diff>
--- a/InventoryManagement/wwwroot/UploadFiles/ProductUpload.xlsx
+++ b/InventoryManagement/wwwroot/UploadFiles/ProductUpload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anujk\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98710E2-E58C-4997-948C-E2D6DA7C862E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0973A2A7-D7FC-4763-AA25-53E7046637F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -45,13 +45,7 @@
     <t>05/05/2024</t>
   </si>
   <si>
-    <t>05/10/2024</t>
-  </si>
-  <si>
-    <t>Book</t>
-  </si>
-  <si>
-    <t>Reading</t>
+    <t>Test25- Blank Created Date and description</t>
   </si>
 </sst>
 </file>
@@ -372,13 +366,15 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -400,19 +396,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>